<commit_message>
add USE CASE + Scénarios
</commit_message>
<xml_diff>
--- a/Journeaux de travaille/Journal_PedroPinto.xlsx
+++ b/Journeaux de travaille/Journal_PedroPinto.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Date</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t xml:space="preserve">Création + Annotation du journal de travaille </t>
+  </si>
+  <si>
+    <t>12h20</t>
+  </si>
+  <si>
+    <t>40min</t>
+  </si>
+  <si>
+    <t>Consseption des USE CASE + Scénarios</t>
   </si>
 </sst>
 </file>
@@ -339,24 +348,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <name val="Arial"/>
-        <scheme val="none"/>
-      </font>
-      <fill>
-        <patternFill>
-          <fgColor indexed="64"/>
-          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -506,24 +497,42 @@
       </border>
     </dxf>
     <dxf>
-      <border>
-        <bottom style="thin">
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="medium">
+          <color indexed="64"/>
+        </left>
+        <right style="medium">
+          <color indexed="64"/>
+        </right>
+        <top style="medium">
+          <color indexed="64"/>
+        </top>
+        <bottom style="medium">
           <color indexed="64"/>
         </bottom>
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="medium">
-          <color indexed="64"/>
-        </left>
-        <right style="medium">
-          <color indexed="64"/>
-        </right>
-        <top style="medium">
-          <color indexed="64"/>
-        </top>
-        <bottom style="medium">
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <name val="Arial"/>
+        <scheme val="none"/>
+      </font>
+      <fill>
+        <patternFill>
+          <fgColor indexed="64"/>
+          <bgColor theme="0" tint="-4.9989318521683403E-2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
           <color indexed="64"/>
         </bottom>
       </border>
@@ -572,14 +581,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau2" displayName="Tableau2" ref="B3:G30" totalsRowShown="0" headerRowDxfId="10" dataDxfId="1" headerRowBorderDxfId="8" tableBorderDxfId="9" totalsRowBorderDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau2" displayName="Tableau2" ref="B3:G30" totalsRowShown="0" headerRowDxfId="10" dataDxfId="8" headerRowBorderDxfId="9" tableBorderDxfId="7" totalsRowBorderDxfId="6">
   <autoFilter ref="B3:G30"/>
   <tableColumns count="6">
-    <tableColumn id="1" name="Date" dataDxfId="6"/>
-    <tableColumn id="2" name="Heure début" dataDxfId="5"/>
-    <tableColumn id="3" name="Heure fin" dataDxfId="4"/>
-    <tableColumn id="4" name="Temps" dataDxfId="3"/>
-    <tableColumn id="5" name="Projet" dataDxfId="2"/>
+    <tableColumn id="1" name="Date" dataDxfId="5"/>
+    <tableColumn id="2" name="Heure début" dataDxfId="4"/>
+    <tableColumn id="3" name="Heure fin" dataDxfId="3"/>
+    <tableColumn id="4" name="Temps" dataDxfId="2"/>
+    <tableColumn id="5" name="Projet" dataDxfId="1"/>
     <tableColumn id="6" name="Déscription" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -851,8 +860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -863,7 +872,7 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.7109375" style="15" customWidth="1"/>
+    <col min="7" max="7" width="42.42578125" style="15" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.5">
@@ -970,12 +979,24 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="10"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="12"/>
-      <c r="G8" s="18"/>
+      <c r="B8" s="9">
+        <v>44232</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="E8" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="18" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B9" s="9"/>

</xml_diff>

<commit_message>
Ajout info dans le JDT
</commit_message>
<xml_diff>
--- a/Journeaux de travaille/Journal_PedroPinto.xlsx
+++ b/Journeaux de travaille/Journal_PedroPinto.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="45">
   <si>
     <t>Date</t>
   </si>
@@ -153,6 +153,24 @@
   </si>
   <si>
     <t>Avancée dans la Documentation principal</t>
+  </si>
+  <si>
+    <t>90min</t>
+  </si>
+  <si>
+    <t>10H00</t>
+  </si>
+  <si>
+    <t>Retour sur la fin du sprinte 1
+et le début du sprinte 2 avec  Mr.Chavais et Simon Cuany</t>
+  </si>
+  <si>
+    <t>Rédaction de l'analyse dans la documentationb 
+avec Simon Cuany</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cloturation du 1er sprinte + envois de l'analyse du projet + Début du 2éme sprint sur le 
+repository </t>
   </si>
 </sst>
 </file>
@@ -217,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -253,44 +271,11 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -306,28 +291,10 @@
     <xf numFmtId="20" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="3" fillId="4" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="20" fontId="3" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -339,17 +306,8 @@
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -373,7 +331,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="left" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -386,6 +344,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -405,7 +369,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -418,6 +382,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -438,7 +408,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -451,6 +421,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -471,7 +447,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -484,6 +460,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -504,7 +486,7 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
@@ -517,6 +499,12 @@
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -537,13 +525,25 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="top" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
+      <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color indexed="64"/>
         </left>
-        <right/>
-        <top/>
-        <bottom/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -917,8 +917,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+    <sheetView tabSelected="1" topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -929,7 +929,7 @@
     <col min="4" max="4" width="11.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="42.42578125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.28515625" style="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="63" customHeight="1" x14ac:dyDescent="0.5">
@@ -953,12 +953,12 @@
       <c r="F3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="10" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:7" s="4" customFormat="1" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="7"/>
+      <c r="B4" s="8"/>
       <c r="C4" s="5" t="s">
         <v>7</v>
       </c>
@@ -968,15 +968,15 @@
       <c r="E4" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="17" t="s">
+      <c r="F4" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="11" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
+      <c r="B5" s="8">
         <v>44230</v>
       </c>
       <c r="C5" s="5" t="s">
@@ -988,15 +988,15 @@
       <c r="E5" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G5" s="17" t="s">
+      <c r="F5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G5" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
+      <c r="B6" s="8">
         <v>44232</v>
       </c>
       <c r="C6" s="5" t="s">
@@ -1008,15 +1008,15 @@
       <c r="E6" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F6" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G6" s="17" t="s">
+      <c r="F6" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" s="11" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B7" s="9">
+      <c r="B7" s="8">
         <v>44232</v>
       </c>
       <c r="C7" s="6" t="s">
@@ -1028,75 +1028,75 @@
       <c r="E7" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G7" s="18" t="s">
+      <c r="F7" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G7" s="12" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B8" s="9">
+      <c r="B8" s="8">
         <v>44232</v>
       </c>
       <c r="C8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G8" s="18" t="s">
+      <c r="F8" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G8" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
+      <c r="B9" s="8">
         <v>44235</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="11" t="s">
+      <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G9" s="19" t="s">
+      <c r="F9" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G9" s="11" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.5" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
+      <c r="B10" s="8">
         <v>44235</v>
       </c>
-      <c r="C10" s="10" t="s">
+      <c r="C10" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D10" s="10" t="s">
+      <c r="D10" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F10" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G10" s="17" t="s">
+      <c r="F10" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="11" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11" s="9">
+      <c r="B11" s="8">
         <v>44235</v>
       </c>
       <c r="C11" s="5" t="s">
@@ -1108,15 +1108,15 @@
       <c r="E11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F11" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G11" s="17" t="s">
+      <c r="F11" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G11" s="11" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="99.75" x14ac:dyDescent="0.25">
-      <c r="B12" s="9">
+      <c r="B12" s="8">
         <v>44235</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1128,192 +1128,250 @@
       <c r="E12" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="F12" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G12" s="17" t="s">
+      <c r="F12" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G12" s="11" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13" s="9">
+      <c r="B13" s="8">
         <v>44239</v>
       </c>
-      <c r="C13" s="10" t="s">
+      <c r="C13" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D13" s="10" t="s">
+      <c r="D13" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="F13" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G13" s="18" t="s">
+      <c r="F13" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14" s="9">
+      <c r="B14" s="8">
         <v>44242</v>
       </c>
-      <c r="C14" s="10" t="s">
+      <c r="C14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D14" s="10" t="s">
+      <c r="D14" s="5" t="s">
         <v>35</v>
       </c>
       <c r="E14" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="F14" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" s="18" t="s">
+      <c r="F14" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" s="12" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15" s="9">
+      <c r="B15" s="8">
         <v>44242</v>
       </c>
-      <c r="C15" s="10" t="s">
+      <c r="C15" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="5" t="s">
         <v>7</v>
       </c>
       <c r="E15" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F15" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="G15" s="17" t="s">
+      <c r="F15" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="11" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B16" s="7"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="12"/>
-      <c r="G16" s="20"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="9"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="20"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="7"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="17"/>
+    <row r="16" spans="1:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>44256</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="F16" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="42.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>44256</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="57" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>44256</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E18" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="F18" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" s="11" t="s">
+        <v>44</v>
+      </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="5"/>
       <c r="D19" s="5"/>
       <c r="E19" s="6"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="17"/>
+      <c r="F19" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" s="11"/>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="11"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="19"/>
+      <c r="B20" s="8"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" s="11"/>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="5"/>
       <c r="D21" s="5"/>
       <c r="E21" s="6"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="20"/>
+      <c r="F21" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="12"/>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B22" s="7"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="5"/>
       <c r="D22" s="5"/>
-      <c r="E22" s="14"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="21"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="11"/>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="19"/>
+      <c r="B23" s="8"/>
+      <c r="C23" s="5"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="6"/>
+      <c r="F23" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="11"/>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="11"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="19"/>
+      <c r="B24" s="8"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G24" s="11"/>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B25" s="9"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="10"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="20"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G25" s="12"/>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B26" s="9"/>
-      <c r="C26" s="10"/>
-      <c r="D26" s="10"/>
-      <c r="E26" s="11"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="20"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G26" s="12"/>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B27" s="9"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="20"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="6"/>
+      <c r="F27" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G27" s="12"/>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="17"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G28" s="11"/>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B29" s="9"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="20"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="5"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="12"/>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B30" s="9"/>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="20"/>
+      <c r="B30" s="8"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="12"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>